<commit_message>
refactor(xlsx): se cambia estructura humcontrato
</commit_message>
<xml_diff>
--- a/src/assets/ejemplos/modelo/HumContrato.xlsx
+++ b/src/assets/ejemplos/modelo/HumContrato.xlsx
@@ -72,11 +72,25 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
+          <t xml:space="preserve">Los valores posibles para este campo son:
+1: Tiempo completo
+2: Medio tiempo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
           <t xml:space="preserve">El formato debe ser tipo texto, el valor no puede llevar ningun punto o signo</t>
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -90,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -104,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -118,7 +132,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -132,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -144,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -156,7 +170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -170,7 +184,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -197,7 +211,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -209,7 +223,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -222,7 +236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="Q1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -236,7 +250,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="R1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -262,7 +276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="S1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -274,7 +288,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0">
+    <comment ref="T1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -286,7 +300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0">
+    <comment ref="U1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -298,7 +312,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="V1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -315,7 +329,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Código empleado</t>
   </si>
@@ -327,6 +341,9 @@
   </si>
   <si>
     <t xml:space="preserve">fecha_hasta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tiempo</t>
   </si>
   <si>
     <t xml:space="preserve">salario</t>
@@ -761,10 +778,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD1048576"/>
+  <dimension ref="A1:W1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U2" activeCellId="0" sqref="U2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -772,23 +789,23 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="5.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="12.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="7.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="5.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="5.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="6.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="11.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="10.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="28.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="9.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="5.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="7.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="5.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="6.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="11.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="14.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="10.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="28.35"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -855,10 +872,12 @@
       <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="XFD1" s="1"/>
+      <c r="W1" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -874,17 +893,17 @@
         <v>20250101</v>
       </c>
       <c r="E2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="n">
         <v>1500000</v>
       </c>
-      <c r="F2" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="G2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H2" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="I2" s="1" t="n">
         <v>1</v>
       </c>
@@ -916,16 +935,19 @@
         <v>1</v>
       </c>
       <c r="S2" s="1" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="T2" s="1" t="n">
         <v>50</v>
       </c>
       <c r="U2" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="V2" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>22</v>
+      <c r="W2" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>